<commit_message>
Delete whitespaces from question_name
</commit_message>
<xml_diff>
--- a/test/xls/partner_data.xlsx
+++ b/test/xls/partner_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
   <si>
     <t>text</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t>Es asociado:</t>
+  </si>
+  <si>
+    <t>type_aux</t>
+  </si>
+  <si>
+    <t>bool</t>
   </si>
 </sst>
 </file>
@@ -528,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -539,14 +545,15 @@
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="3" max="3" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
+    <row r="1" spans="1:10" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -557,25 +564,28 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -585,11 +595,11 @@
       <c r="C2" t="s">
         <v>41</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -600,7 +610,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -611,18 +621,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="8" customFormat="1">
+    <row r="5" spans="1:10" s="8" customFormat="1">
       <c r="A5" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="J5" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="8" customFormat="1">
+    <row r="6" spans="1:10" s="8" customFormat="1">
       <c r="A6" s="7" t="s">
         <v>0</v>
       </c>
@@ -632,11 +642,11 @@
       <c r="C6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="8">
+      <c r="G6" s="8">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="8" customFormat="1">
+    <row r="7" spans="1:10" s="8" customFormat="1">
       <c r="A7" s="7" t="s">
         <v>0</v>
       </c>
@@ -646,11 +656,11 @@
       <c r="C7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="8">
+      <c r="G7" s="8">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="8" customFormat="1">
+    <row r="8" spans="1:10" s="8" customFormat="1">
       <c r="A8" s="10" t="s">
         <v>37</v>
       </c>
@@ -658,7 +668,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="5" customFormat="1">
+    <row r="9" spans="1:10" s="5" customFormat="1">
       <c r="A9" s="5" t="s">
         <v>29</v>
       </c>
@@ -668,11 +678,14 @@
       <c r="C9" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="D9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
@@ -682,6 +695,7 @@
       <c r="C10" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="D10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>